<commit_message>
Rectification de la diffusion
</commit_message>
<xml_diff>
--- a/ecoliModel/init.xlsx
+++ b/ecoliModel/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Emma\Stage_GB5_LBBE\LBBEModelisation\ecoliModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16076E33-C401-426B-900D-E44514303DE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1770CD8E-4762-40C1-8054-BE36095FAABD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metabolites" sheetId="1" r:id="rId1"/>
@@ -949,7 +949,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1054,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1096,6 +1096,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1411,13 +1414,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1580,7 +1585,7 @@
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="15" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1772,7 +1777,7 @@
       <c r="A44" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="15" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1924,7 +1929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2590,7 +2595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3079,7 +3084,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3568,7 +3573,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3641,7 +3646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3706,7 +3711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>